<commit_message>
Connection to DynamoDB using PynamoDB
</commit_message>
<xml_diff>
--- a/docs/Tables.xlsx
+++ b/docs/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\Repositorios\Simple IoT Server\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12603A11-DA9B-440D-95BC-ABB7E534EDD8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA21ABD3-4736-4C35-ACFC-5BB77B3170D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{DBB924BD-98B3-4A2D-ACA3-C3778F84A548}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>id*</t>
   </si>
   <si>
-    <t>type**</t>
-  </si>
-  <si>
     <t>write_key</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>group*</t>
+  </si>
+  <si>
+    <t>type***</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="B2:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -644,63 +644,63 @@
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="O7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -708,31 +708,31 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -740,57 +740,57 @@
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -812,13 +812,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -840,13 +840,13 @@
         <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -854,13 +854,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -868,31 +868,31 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>